<commit_message>
all files after edit
</commit_message>
<xml_diff>
--- a/BOM/MyCustom_75Keeb.xlsx
+++ b/BOM/MyCustom_75Keeb.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer Development\Hardware\65% Keybaord\MyCustom_75Keeb\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2EC4AA-2B16-4A57-9D1C-203E14A5289A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C52BCF72-0BB4-46FA-8542-435842332862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="MyCustom_75Keeb" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
   <si>
     <t>Id</t>
   </si>
@@ -28,60 +41,12 @@
     <t>Designator</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
     <t>Designation</t>
   </si>
   <si>
-    <t>Supplier and ref</t>
-  </si>
-  <si>
-    <t>SW70,SW81,SW19,SW66,SW65,SW33,SW56,SW3,SW77,SW11,SW15,SW29,SW32,SW44,SW40,SW71,SW30,SW1,SW12,SW47,SW73,SW54,SW74,SW59,SW26,SW23,SW37,SW2,SW43,SW36,SW20,SW69,SW4,SW46,SW18,SW50,SW53,SW67,SW35,SW38,SW17,SW60,SW28,SW21,SW68,SW41,SW55,SW58,SW64,SW63,SW13,SW39,SW61,SW48,SW82,SW52,SW25,SW24,SW76,SW7,SW75,SW42,SW83,SW49,SW9,SW84,SW6,SW78,SW22,SW80,SW16,SW8,SW34,SW62,SW31,SW79,SW5,SW14,SW10,SW51,SW27,SW45,SW72,SW57</t>
-  </si>
-  <si>
-    <t>SW_Cherry_MX_PCB_1.00u</t>
-  </si>
-  <si>
-    <t>SW_Push_45deg</t>
-  </si>
-  <si>
-    <t>S6</t>
-  </si>
-  <si>
-    <t>STAB_MX_P_2u</t>
-  </si>
-  <si>
-    <t>MX_stab</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>STAB_MX_P_2.25u</t>
-  </si>
-  <si>
-    <t>S5</t>
-  </si>
-  <si>
-    <t>STAB_MX_2u</t>
-  </si>
-  <si>
-    <t>S7</t>
-  </si>
-  <si>
-    <t>STAB_MX_2.25u</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>STAB_MX_P_6.25u</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -203,25 +168,144 @@
   </si>
   <si>
     <t>SW_Push</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/2790619-USBLC62SC6/C2687116</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Nexperia-74LVCH2T45DC125/C548924</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/STMicroelectronics-STM32F072CBT6/C81720</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/1877-CL05B104KO5NNNC/C1525</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/TorexSemicon-XC6206P332MRG/C5446</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/15869-CL05B103KB5NNNC/C15195</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/26487-0402WGF1002TCE/C25744</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/24469-CL05A475MP5NRNC/C23733</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/OPSCOOptoelectronics-SK6812MINIE/C5149201</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/53938-CL05A105KA5NQNC/C52923</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Hongda-2009T500mA250V/C529783</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Alpsalpine-SKQGABE010/C115351</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Comchip-CZRU52C2V7HF/C2886070</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Korean_HropartsElec-TYPE_C_31_M12/C165948</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/26648-0402WGF5101TCE/C25905</t>
+  </si>
+  <si>
+    <t>https://www.amazon.eg/-/en/GATERON-Switches-Pre-lubed-Mechanical-Keyboard/dp/B0C65CVFMV/ref=sr_1_1?crid=35S9XGI0ENMXB&amp;dib=eyJ2IjoiMSJ9.d0rbggVbkY0AcsIOwnBzFNULdphzE6W0rlyz1HhG5tNSrqc6oCjKiMMfAGdBwejhOlkNgiInz75ECy8O06KforDjZA233jd8GNoxoh39m_SqIkaW26QnkThHkkhlB1ZI-B_8fgqF_hGCQPZztyn-d_icpNZ93Mic3pYLI0S80ToPgStGJqp4SO92OJSYXLJKqpl--ocsgzHtjhqEM8eV2YaUhACyUSxQeadWLHBYYOP253VaDb_kpyBg578KGPHhJ4UHjX52Yc2h2d-DgqUTfEFFnpyuwljG12E6-Kc1pjw.2cwQPqlwwLG7Na5cXEqxRVIz7qc4jVd8Jm9gclFc0jg&amp;dib_tag=se&amp;keywords=rgb+switches&amp;qid=1764881966&amp;sprefix=rgb+switche%2Caps%2C116&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>GATERON G Pro 3.0 Switches Pre-lubed 5 pinS RGB Linear for Gaming Mechanical Keyboard (Yellow)</t>
+  </si>
+  <si>
+    <t>Footprint PCB ONLY</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Supplier (LINK)</t>
+  </si>
+  <si>
+    <t>Redragon A101 Replacement Keycaps,104 Keyboard Keycaps, Compatible, Mechanical Keyboard Keycaps Inclusive Keypuller for Mechanical Keyboard || White</t>
+  </si>
+  <si>
+    <t>https://www.amazon.eg/-/en/Redragon-Replacement-Compatible-Mechanical-Inclusive/dp/B01A574S82/ref=sr_1_1?crid=2L60MJ7PPE097&amp;dib=eyJ2IjoiMSJ9.KyI_7CGlbZhr6NDzrMTj7w3asZ5RSBzZwEFuJR78WSLMUJ73iaPLwEV-Cp5FdvAd3MR2DkHI4jUgVw7XOc7u-qXMEKT6wlpqoC5JsHeYxC4Gj1TiC1o1MuF7g3UUrkA3psefb5vmsL3PTTkMxGFPTYJdYBygHcIJCESxAmPNnimXeCMWxx8EuDquKGwW_aWAT0txQWCJ4YYfK8LVMn2RYi7uy4tvK8g1HXTDJyyDPAWWwfOdlVBR30HJyBcllohBMztxqIolNp5tOzoRgXTXUedBP8LolIOs_cbRc0W9n_0.uhbGyxkaR5UnQn3JBofuu-GOld6ZE45fhiGsv6S-hXg&amp;dib_tag=se&amp;keywords=key+caps&amp;qid=1764882121&amp;sprefix=key+cap%2Caps%2C116&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>TOTAL IN USD</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>PCB 5 pics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0F1111"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF8C22"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CC00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -233,13 +317,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,9 +642,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -553,387 +655,513 @@
     <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="19.109375" customWidth="1"/>
     <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
+      <c r="F1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="5">
+        <v>12.63</v>
+      </c>
+      <c r="I6" s="5">
+        <v>12.63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
+      <c r="B7" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="5">
+        <v>10.52</v>
+      </c>
+      <c r="I7" s="5">
+        <v>10.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="I8">
+        <f>PRODUCT(G8,D8)</f>
+        <v>0.56399999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>84</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9">
+        <v>5.7799999999999997E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:I22" si="0">PRODUCT(G9,D9)</f>
+        <v>4.8552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>84</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>3.6799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>2.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16">
+        <v>1.3005</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>1.3005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <v>1.4E-3</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19">
+        <v>9.98E-2</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>9.98E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21">
+        <v>5.5100000000000003E-2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>5.5100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>44</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25">
+        <f>SUM(I8:I22)</f>
+        <v>12.145900000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.4">
+      <c r="A26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="I26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G27" s="7"/>
+      <c r="I27">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <hyperlinks>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{3D952FDF-31BC-43B1-BECB-A2FA49D6721B}"/>
+    <hyperlink ref="F22" r:id="rId2" xr:uid="{A1B1E27C-775C-415E-AC5F-2E924C7DCDB3}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{5001F1FC-3179-4E89-A203-7CFF5089C7CA}"/>
+    <hyperlink ref="F13" r:id="rId4" xr:uid="{AA6D5B53-7A44-4BCB-BB03-97A4B9CB976B}"/>
+    <hyperlink ref="F12" r:id="rId5" xr:uid="{F4062A57-D1BB-405C-AB72-E3583051D995}"/>
+    <hyperlink ref="F11" r:id="rId6" xr:uid="{655982F1-3220-4878-9C34-4151507EC320}"/>
+    <hyperlink ref="F17" r:id="rId7" xr:uid="{C653804C-198A-43A2-A278-E86E91A88B17}"/>
+    <hyperlink ref="F18" r:id="rId8" xr:uid="{5C85943B-C940-42B0-9A73-6D37AB4E57A9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>